<commit_message>
minor cleanups to block diagram
</commit_message>
<xml_diff>
--- a/Scope & Calculations/MOSFET Switching Times Calculator.xlsx
+++ b/Scope & Calculations/MOSFET Switching Times Calculator.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Farris' Files\School\Side Projects\Electric Scooter\custom-escooter\Scope &amp; Calculations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32A601C7-DA3A-4205-9070-9FB675D8C183}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8969535E-BEE3-4C2D-AA06-4D419C15C273}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="NTMTS001N06CTXG" sheetId="1" r:id="rId1"/>
-    <sheet name="NVMFS5C628NWFT1G " sheetId="3" r:id="rId2"/>
-    <sheet name="NVMFS5C628NWFT1G (2)" sheetId="2" r:id="rId3"/>
+    <sheet name="CSD18540Q5B" sheetId="4" r:id="rId1"/>
+    <sheet name="NTMTS001N06CTXG" sheetId="1" r:id="rId2"/>
+    <sheet name="NVMFS5C628NWFT1G " sheetId="3" r:id="rId3"/>
+    <sheet name="NVMFS5C628NWFT1G (2)" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="22">
   <si>
     <t>Datasheet Parameters</t>
   </si>
@@ -438,6 +439,180 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60C9ED18-D1AD-4826-B7A9-FE34018C60F3}">
+  <dimension ref="A1:H11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="D1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="2"/>
+      <c r="G1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" s="2"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>0.8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2">
+        <v>43.2</v>
+      </c>
+      <c r="G2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2">
+        <f>(B2+E5)*B4*10^-12*LN(1/(1-B6/E7))*10^9 + (B2+E5)*B4*10^-12*LN((E7-B6)/(E7-B7))*10^9</f>
+        <v>8.0349292901555369</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>6.7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3">
+        <v>36</v>
+      </c>
+      <c r="G3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3">
+        <f>(B2+E5)*B3*10^-9*E2/E8/(E7-B7)*10^9</f>
+        <v>5.1163636363636362</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4">
+        <v>3200</v>
+      </c>
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4">
+        <v>200</v>
+      </c>
+      <c r="G4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H4">
+        <f>(B2+E6)*B5*10^-12*LN(E7/B7)*10^9</f>
+        <v>5.0305984861719608</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5">
+        <v>3500</v>
+      </c>
+      <c r="D5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5">
+        <v>3.4</v>
+      </c>
+      <c r="G5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H5">
+        <f>(B2+E6)*B3*10^-9*E2/E8/B7*10^9</f>
+        <v>2.6799999999999997</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6">
+        <v>1.9</v>
+      </c>
+      <c r="D6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7">
+        <v>4.5</v>
+      </c>
+      <c r="D7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8">
+        <v>43.2</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H8" s="1">
+        <f>SUM(H2:H5)*10^-9*0.5*E2*E3*E4*10^3</f>
+        <v>3.2444413525017253</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="G1:H1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H8"/>
   <sheetViews>
@@ -605,12 +780,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{275AFA95-BF28-447F-A146-DCF296D31718}">
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -779,7 +954,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C23B407-03D2-43A6-B0FB-4D90FFED92FB}">
   <dimension ref="A1:H11"/>
   <sheetViews>

</xml_diff>

<commit_message>
BC-MPR: added power stage for bidirectional buck-boost
</commit_message>
<xml_diff>
--- a/Scope & Calculations/MOSFET Switching Times Calculator.xlsx
+++ b/Scope & Calculations/MOSFET Switching Times Calculator.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Farris' Files\School\Side Projects\Electric Scooter\custom-escooter\Scope &amp; Calculations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8969535E-BEE3-4C2D-AA06-4D419C15C273}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01B7B08A-F06A-4370-98AC-D7ED11086F49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="CSD18540Q5B" sheetId="4" r:id="rId1"/>
-    <sheet name="NTMTS001N06CTXG" sheetId="1" r:id="rId2"/>
-    <sheet name="NVMFS5C628NWFT1G " sheetId="3" r:id="rId3"/>
-    <sheet name="NVMFS5C628NWFT1G (2)" sheetId="2" r:id="rId4"/>
+    <sheet name="SQJQ160E-T1_GE3" sheetId="5" r:id="rId1"/>
+    <sheet name="CSD18540Q5B" sheetId="4" r:id="rId2"/>
+    <sheet name="NTMTS001N06CTXG" sheetId="1" r:id="rId3"/>
+    <sheet name="NVMFS5C628NWFT1G " sheetId="3" r:id="rId4"/>
+    <sheet name="NVMFS5C628NWFT1G (2)" sheetId="2" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="22">
   <si>
     <t>Datasheet Parameters</t>
   </si>
@@ -439,11 +440,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60C9ED18-D1AD-4826-B7A9-FE34018C60F3}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B289D3B7-6CDA-4BB4-98DB-B249A0215CBF}">
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -473,7 +474,7 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>0.8</v>
+        <v>1.4</v>
       </c>
       <c r="D2" t="s">
         <v>5</v>
@@ -486,7 +487,7 @@
       </c>
       <c r="H2">
         <f>(B2+E5)*B4*10^-12*LN(1/(1-B6/E7))*10^9 + (B2+E5)*B4*10^-12*LN((E7-B6)/(E7-B7))*10^9</f>
-        <v>8.0349292901555369</v>
+        <v>25.718598592326639</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -494,7 +495,7 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>6.7</v>
+        <v>42</v>
       </c>
       <c r="D3" t="s">
         <v>6</v>
@@ -507,7 +508,7 @@
       </c>
       <c r="H3">
         <f>(B2+E5)*B3*10^-9*E2/E8/(E7-B7)*10^9</f>
-        <v>5.1163636363636362</v>
+        <v>26.88</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -515,7 +516,7 @@
         <v>16</v>
       </c>
       <c r="B4">
-        <v>3200</v>
+        <v>11400</v>
       </c>
       <c r="D4" t="s">
         <v>7</v>
@@ -528,7 +529,7 @@
       </c>
       <c r="H4">
         <f>(B2+E6)*B5*10^-12*LN(E7/B7)*10^9</f>
-        <v>5.0305984861719608</v>
+        <v>32.955862901193996</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -536,7 +537,7 @@
         <v>17</v>
       </c>
       <c r="B5">
-        <v>3500</v>
+        <v>14000</v>
       </c>
       <c r="D5" t="s">
         <v>20</v>
@@ -549,7 +550,7 @@
       </c>
       <c r="H5">
         <f>(B2+E6)*B3*10^-9*E2/E8/B7*10^9</f>
-        <v>2.6799999999999997</v>
+        <v>22.400000000000002</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -557,7 +558,7 @@
         <v>8</v>
       </c>
       <c r="B6">
-        <v>1.9</v>
+        <v>3</v>
       </c>
       <c r="D6" t="s">
         <v>19</v>
@@ -577,7 +578,7 @@
         <v>14</v>
       </c>
       <c r="E7">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -592,7 +593,7 @@
       </c>
       <c r="H8" s="1">
         <f>SUM(H2:H5)*10^-9*0.5*E2*E3*E4*10^3</f>
-        <v>3.2444413525017253</v>
+        <v>16.789077851472332</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -613,11 +614,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60C9ED18-D1AD-4826-B7A9-FE34018C60F3}">
+  <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -647,20 +648,20 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>1.5</v>
+        <v>0.8</v>
       </c>
       <c r="D2" t="s">
         <v>5</v>
       </c>
       <c r="E2">
-        <v>36</v>
+        <v>43.2</v>
       </c>
       <c r="G2" t="s">
         <v>10</v>
       </c>
       <c r="H2">
         <f>(B2+E5)*B4*10^-12*LN(1/(1-B6/E7))*10^9 + (B2+E5)*B4*10^-12*LN((E7-B6)/(E7-B7))*10^9</f>
-        <v>21.973166567159236</v>
+        <v>6.3168487770626855</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -668,7 +669,7 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>16.3</v>
+        <v>6.7</v>
       </c>
       <c r="D3" t="s">
         <v>6</v>
@@ -681,7 +682,7 @@
       </c>
       <c r="H3">
         <f>(B2+E5)*B3*10^-9*E2/E8/(E7-B7)*10^9</f>
-        <v>12.000500834724541</v>
+        <v>3.7520000000000002</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -689,7 +690,7 @@
         <v>16</v>
       </c>
       <c r="B4">
-        <v>8750</v>
+        <v>3200</v>
       </c>
       <c r="D4" t="s">
         <v>7</v>
@@ -702,7 +703,7 @@
       </c>
       <c r="H4">
         <f>(B2+E6)*B5*10^-12*LN(E7/B7)*10^9</f>
-        <v>22.844846291889194</v>
+        <v>6.1792242939738751</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -710,7 +711,7 @@
         <v>17</v>
       </c>
       <c r="B5">
-        <v>10000</v>
+        <v>3500</v>
       </c>
       <c r="D5" t="s">
         <v>20</v>
@@ -723,7 +724,7 @@
       </c>
       <c r="H5">
         <f>(B2+E6)*B3*10^-9*E2/E8/B7*10^9</f>
-        <v>9.1458852867830434</v>
+        <v>2.6799999999999997</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -731,7 +732,7 @@
         <v>8</v>
       </c>
       <c r="B6">
-        <v>3</v>
+        <v>1.9</v>
       </c>
       <c r="D6" t="s">
         <v>19</v>
@@ -745,13 +746,13 @@
         <v>4</v>
       </c>
       <c r="B7">
-        <v>4.01</v>
+        <v>4.5</v>
       </c>
       <c r="D7" t="s">
         <v>14</v>
       </c>
       <c r="E7">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -759,15 +760,21 @@
         <v>15</v>
       </c>
       <c r="E8">
-        <v>40</v>
+        <v>43.2</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>18</v>
       </c>
       <c r="H8" s="1">
         <f>SUM(H2:H5)*10^-9*0.5*E2*E3*E4*10^3</f>
-        <v>8.548986107880058</v>
-      </c>
+        <v>2.9436939240076065</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -781,10 +788,178 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="D1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="2"/>
+      <c r="G1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" s="2"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>1.5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2">
+        <v>36</v>
+      </c>
+      <c r="G2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2">
+        <f>(B2+E5)*B4*10^-12*LN(1/(1-B6/E7))*10^9 + (B2+E5)*B4*10^-12*LN((E7-B6)/(E7-B7))*10^9</f>
+        <v>21.973166567159236</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>16.3</v>
+      </c>
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3">
+        <v>36</v>
+      </c>
+      <c r="G3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3">
+        <f>(B2+E5)*B3*10^-9*E2/E8/(E7-B7)*10^9</f>
+        <v>12.000500834724541</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4">
+        <v>8750</v>
+      </c>
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4">
+        <v>200</v>
+      </c>
+      <c r="G4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H4">
+        <f>(B2+E6)*B5*10^-12*LN(E7/B7)*10^9</f>
+        <v>22.844846291889194</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5">
+        <v>10000</v>
+      </c>
+      <c r="D5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5">
+        <v>3.4</v>
+      </c>
+      <c r="G5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H5">
+        <f>(B2+E6)*B3*10^-9*E2/E8/B7*10^9</f>
+        <v>9.1458852867830434</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6">
+        <v>3</v>
+      </c>
+      <c r="D6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7">
+        <v>4.01</v>
+      </c>
+      <c r="D7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8">
+        <v>40</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H8" s="1">
+        <f>SUM(H2:H5)*10^-9*0.5*E2*E3*E4*10^3</f>
+        <v>8.548986107880058</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="G1:H1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{275AFA95-BF28-447F-A146-DCF296D31718}">
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
@@ -954,7 +1129,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C23B407-03D2-43A6-B0FB-4D90FFED92FB}">
   <dimension ref="A1:H11"/>
   <sheetViews>

</xml_diff>